<commit_message>
Align with changed table schema
</commit_message>
<xml_diff>
--- a/Documents/Skool_Web.xlsx
+++ b/Documents/Skool_Web.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>Page</t>
   </si>
@@ -44,96 +44,12 @@
     <t>Employee</t>
   </si>
   <si>
-    <t>EmpId</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>ISD Information</t>
-  </si>
-  <si>
-    <t>LN Id</t>
-  </si>
-  <si>
-    <t>IBM DOJ</t>
-  </si>
-  <si>
-    <t>Account DOJ</t>
-  </si>
-  <si>
-    <t>Role Id</t>
-  </si>
-  <si>
-    <t>Band ID</t>
-  </si>
-  <si>
-    <t>Team Id</t>
-  </si>
-  <si>
-    <t>Team Name</t>
-  </si>
-  <si>
-    <t>User Team</t>
-  </si>
-  <si>
-    <t>userid</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>Userid</t>
-  </si>
-  <si>
-    <t>Teamid</t>
-  </si>
-  <si>
     <t>TierId</t>
   </si>
   <si>
-    <t>OverAll Score</t>
-  </si>
-  <si>
     <t>EmpId, Name,ISD Information,LN Id,IBM DOJ,Account DOJ,Role Name,Band ,IBM Teanure, Accout Tenure,OverAll Score, Tier</t>
   </si>
   <si>
-    <t>table_TeamMaster</t>
-  </si>
-  <si>
-    <t>table_UserMaster</t>
-  </si>
-  <si>
-    <t>table_RoleMaster</t>
-  </si>
-  <si>
-    <t>roleid</t>
-  </si>
-  <si>
-    <t>rolename</t>
-  </si>
-  <si>
-    <t>table_BandMaster</t>
-  </si>
-  <si>
-    <t>bandid</t>
-  </si>
-  <si>
-    <t>bandname</t>
-  </si>
-  <si>
-    <t>table_tierMaster</t>
-  </si>
-  <si>
-    <t>tierid</t>
-  </si>
-  <si>
-    <t>tirename</t>
-  </si>
-  <si>
     <t>API</t>
   </si>
   <si>
@@ -176,33 +92,6 @@
     <t>TeamId</t>
   </si>
   <si>
-    <t>Primary Skill</t>
-  </si>
-  <si>
-    <t>Primary Skill Score</t>
-  </si>
-  <si>
-    <t>SecondarySkillWeight</t>
-  </si>
-  <si>
-    <t>TertiarySkillWeight</t>
-  </si>
-  <si>
-    <t>Primary skill weight</t>
-  </si>
-  <si>
-    <t>SecondarySkill</t>
-  </si>
-  <si>
-    <t>SecondarySkillScore</t>
-  </si>
-  <si>
-    <t>TertiarySkill</t>
-  </si>
-  <si>
-    <t>TertiarySkillScore</t>
-  </si>
-  <si>
     <t>Group</t>
   </si>
   <si>
@@ -251,9 +140,6 @@
     <t>AttributeId</t>
   </si>
   <si>
-    <t>Attribute_GroupId</t>
-  </si>
-  <si>
     <t>AttributeName</t>
   </si>
   <si>
@@ -270,13 +156,193 @@
   </si>
   <si>
     <t>EmployeeTeamAttribute_AttributeId</t>
+  </si>
+  <si>
+    <t>JobRole</t>
+  </si>
+  <si>
+    <t>JobRoleId</t>
+  </si>
+  <si>
+    <t>JobRole_TeamId</t>
+  </si>
+  <si>
+    <t>EmployeeName</t>
+  </si>
+  <si>
+    <t>EmployeeTeamAttributeValue</t>
+  </si>
+  <si>
+    <t>JobRoleGroup</t>
+  </si>
+  <si>
+    <t>JobRoleGroupId</t>
+  </si>
+  <si>
+    <t>JobRoleGroup_GroupId</t>
+  </si>
+  <si>
+    <t>JobRoleGroup_JobRoleId</t>
+  </si>
+  <si>
+    <t>EmployeeLNId</t>
+  </si>
+  <si>
+    <t>EmployeeIBMDOJ</t>
+  </si>
+  <si>
+    <t>EmployeeAccountDOJ</t>
+  </si>
+  <si>
+    <t>Employee_BandID</t>
+  </si>
+  <si>
+    <t>Band</t>
+  </si>
+  <si>
+    <t>BandId</t>
+  </si>
+  <si>
+    <t>BandName</t>
+  </si>
+  <si>
+    <t>RoleId</t>
+  </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>UserTeam</t>
+  </si>
+  <si>
+    <t>TeamName</t>
+  </si>
+  <si>
+    <t>EmployeeTeamId</t>
+  </si>
+  <si>
+    <t>EmployeeTeam_EmployeeId</t>
+  </si>
+  <si>
+    <t>EmployeeTeam_TeamId</t>
+  </si>
+  <si>
+    <t>EmployeeTeam_RoleId</t>
+  </si>
+  <si>
+    <t>EmployeeTeam_TierId</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Tier</t>
+  </si>
+  <si>
+    <t>TireName</t>
+  </si>
+  <si>
+    <t>EmployeeTeamGroup</t>
+  </si>
+  <si>
+    <t>EmployeeTeamGroupId</t>
+  </si>
+  <si>
+    <t>EmployeeTeamGroup_EmployeeTeamId</t>
+  </si>
+  <si>
+    <t>EmployeeTeamGroup_GroupId</t>
+  </si>
+  <si>
+    <t>EmployeeTeamGroupApplicationScore</t>
+  </si>
+  <si>
+    <t>EmployeeTeamGroupRolewiseWeight</t>
+  </si>
+  <si>
+    <t>EmployeeTeamGroupTargetScore</t>
+  </si>
+  <si>
+    <t>EmployeeTeamGroupRolewiseScore</t>
+  </si>
+  <si>
+    <t>Attribute_JobRoleGroupId</t>
+  </si>
+  <si>
+    <t>EmployeeTeamOverAllScore</t>
+  </si>
+  <si>
+    <t>EmployeeTeamPrimarySkill_TeamTechnologyId</t>
+  </si>
+  <si>
+    <t>EmployeeTeamPrimarySkillScore</t>
+  </si>
+  <si>
+    <t>EmployeeTeamPrimarySkillWeight</t>
+  </si>
+  <si>
+    <t>EmployeeTeamSecondarySkillScore</t>
+  </si>
+  <si>
+    <t>EmployeeTeamSecondarySkillWeight</t>
+  </si>
+  <si>
+    <t>EmployeeTeamTertiarySkillScore</t>
+  </si>
+  <si>
+    <t>EmployeeTeamTertiarySkillWeight</t>
+  </si>
+  <si>
+    <t>EmployeeTeamSecondarySkill_TeamTechnologyId</t>
+  </si>
+  <si>
+    <t>EmployeeTeamTertiarySkill__TeamTechnologyId</t>
+  </si>
+  <si>
+    <t>JobRoleName</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>UserPassword</t>
+  </si>
+  <si>
+    <t>UserEmail</t>
+  </si>
+  <si>
+    <t>UserTeamId</t>
+  </si>
+  <si>
+    <t>UserTeam_TeamId</t>
+  </si>
+  <si>
+    <t>UserTeam_UserId</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>EmployeeJobType</t>
+  </si>
+  <si>
+    <t>EmployeeJobTypeId</t>
+  </si>
+  <si>
+    <t>EmployeeJobTypeName</t>
+  </si>
+  <si>
+    <t>Employee_EmployeeJobTypeId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,8 +350,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,6 +387,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -406,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -415,12 +495,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -435,18 +509,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -775,70 +860,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="13">
+      <c r="A1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="11">
         <v>42817</v>
       </c>
-      <c r="C1" s="13">
+      <c r="C1" s="11">
         <v>42818</v>
       </c>
-      <c r="D1" s="13">
+      <c r="D1" s="11">
         <v>42821</v>
       </c>
-      <c r="E1" s="13">
+      <c r="E1" s="11">
         <v>42822</v>
       </c>
-      <c r="F1" s="13">
+      <c r="F1" s="11">
         <v>42823</v>
       </c>
-      <c r="G1" s="13">
+      <c r="G1" s="11">
         <v>42824</v>
       </c>
-      <c r="H1" s="13">
+      <c r="H1" s="11">
         <v>42825</v>
       </c>
-      <c r="I1" s="13">
+      <c r="I1" s="11">
         <v>42826</v>
       </c>
-      <c r="J1" s="13">
+      <c r="J1" s="11">
         <v>42827</v>
       </c>
-      <c r="K1" s="13">
+      <c r="K1" s="11">
         <v>42828</v>
       </c>
-      <c r="L1" s="13">
+      <c r="L1" s="11">
         <v>42829</v>
       </c>
-      <c r="M1" s="13">
+      <c r="M1" s="11">
         <v>42830</v>
       </c>
-      <c r="N1" s="13">
+      <c r="N1" s="11">
         <v>42831</v>
       </c>
-      <c r="O1" s="13">
+      <c r="O1" s="11">
         <v>42832</v>
       </c>
-      <c r="P1" s="13">
+      <c r="P1" s="11">
         <v>42833</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+        <v>15</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+        <v>16</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -888,347 +973,470 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L24"/>
+  <dimension ref="B1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="E2" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="21"/>
-      <c r="H2" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="21"/>
-      <c r="K2" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" s="17"/>
+      <c r="C2" s="24"/>
+      <c r="E2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="H2" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="24"/>
+      <c r="K2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="24"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3"/>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F3" s="3"/>
       <c r="H3" s="2" t="s">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="I3" s="3"/>
       <c r="K3" s="2" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="C4" s="3"/>
       <c r="E4" s="4" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="H4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="5"/>
+      <c r="H4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" s="3"/>
       <c r="K4" s="2" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="C5" s="3"/>
+      <c r="H5" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" s="5"/>
       <c r="K5" s="2" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="E6" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="21"/>
-      <c r="H6" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="21"/>
+      <c r="E6" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="24"/>
       <c r="K6" s="2" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="L6" s="3"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="C7" s="3"/>
       <c r="E7" s="2" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="H7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="3"/>
+      <c r="H7" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="I7" s="24"/>
       <c r="K7" s="2" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="C8" s="3"/>
       <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="H8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="5"/>
+      <c r="H8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="3"/>
       <c r="K8" s="2" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="L8" s="3"/>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="C9" s="5"/>
       <c r="E9" s="4" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="F9" s="5"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="H9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="5"/>
       <c r="K9" s="2" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="H10" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="21"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
       <c r="K10" s="2" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="E11" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="21"/>
-      <c r="H11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="3"/>
+      <c r="B11" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="E11" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="H11" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="24"/>
       <c r="K11" s="2" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="C12" s="3"/>
       <c r="E12" s="2" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="H12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" s="5"/>
+      <c r="H12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="3"/>
       <c r="K12" s="2" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="C13" s="5"/>
       <c r="E13" s="4" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="F13" s="5"/>
+      <c r="H13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="5"/>
       <c r="K13" s="2" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K14" s="2" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="E15" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="21"/>
-      <c r="H15" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="I15" s="21"/>
+      <c r="B15" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="E15" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="24"/>
+      <c r="H15" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="24"/>
       <c r="K15" s="2" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="3"/>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="17"/>
       <c r="E16" s="2" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="F16" s="3"/>
       <c r="H16" s="2" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="I16" s="3"/>
-      <c r="K16" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L16" s="5"/>
-    </row>
-    <row r="17" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="3"/>
+      <c r="K16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="17"/>
       <c r="E17" s="4" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="F17" s="5"/>
       <c r="H17" s="2" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" s="5"/>
+      <c r="K17" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="19"/>
       <c r="H18" s="2" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="21"/>
+    <row r="19" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="24"/>
       <c r="H19" s="4" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="24"/>
       <c r="E20" s="2" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="3"/>
       <c r="E21" s="2" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="H21" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="I21" s="21"/>
-    </row>
-    <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="26"/>
+    </row>
+    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="3"/>
       <c r="E22" s="4" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="F22" s="5"/>
       <c r="H22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="H23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="24"/>
+      <c r="H24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="24"/>
+      <c r="E25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="H25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="E26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="E27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="E28" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="E29" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="24"/>
+      <c r="E30" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="E31" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H23" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H24" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I24" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="20"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="20"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="H21:I21"/>
+  <mergeCells count="17">
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="E19:F19"/>
-    <mergeCell ref="H15:I15"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E6:F6"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H7:I7"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1251,36 +1459,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>37</v>
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>40</v>
+      <c r="A2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>23</v>
+      <c r="A3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
latest update from jaydeep 17 Jun 2017
</commit_message>
<xml_diff>
--- a/Documents/Skool_Web.xlsx
+++ b/Documents/Skool_Web.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19365" windowHeight="9270" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19365" windowHeight="9270" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="4" r:id="rId1"/>
     <sheet name="Pages" sheetId="1" r:id="rId2"/>
     <sheet name="DataBase" sheetId="3" r:id="rId3"/>
-    <sheet name="Api" sheetId="2" r:id="rId4"/>
+    <sheet name="DB2" sheetId="5" r:id="rId4"/>
+    <sheet name="Api" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="119">
   <si>
     <t>Page</t>
   </si>
@@ -339,6 +340,51 @@
   </si>
   <si>
     <t>EmployeeTeamTertiarySkill_TeamTechnologyId</t>
+  </si>
+  <si>
+    <t>EmployeeTeam_JobRoleId</t>
+  </si>
+  <si>
+    <t>EmployeeFieldMaster</t>
+  </si>
+  <si>
+    <t>EmployeeFieldMasterId</t>
+  </si>
+  <si>
+    <t>EmployeeFieldMasterField</t>
+  </si>
+  <si>
+    <t>EmployeeFieldMasterIsVisible</t>
+  </si>
+  <si>
+    <t>EmployeeFieldMaster_JobRoleGroupId</t>
+  </si>
+  <si>
+    <t>EmployeeMeta</t>
+  </si>
+  <si>
+    <t>EmployeeMetaId</t>
+  </si>
+  <si>
+    <t>EmployeeMeta_EmployeeId</t>
+  </si>
+  <si>
+    <t>EmployeeMeta_Key</t>
+  </si>
+  <si>
+    <t>EmployeeMeta_Value</t>
+  </si>
+  <si>
+    <t>EmployeeMetaYear</t>
+  </si>
+  <si>
+    <t>EmployeeMetaQuarter</t>
+  </si>
+  <si>
+    <t>EmployeeMetaCreated</t>
+  </si>
+  <si>
+    <t>EmployeeMetaLastModified</t>
   </si>
 </sst>
 </file>
@@ -489,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -535,6 +581,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -978,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,9 +1046,9 @@
     <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" customWidth="1"/>
-    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="50.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1246,10 +1305,10 @@
         <v>79</v>
       </c>
       <c r="I17" s="3"/>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="L17" s="5"/>
+      <c r="L17" s="3"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="16" t="s">
@@ -1260,6 +1319,10 @@
         <v>37</v>
       </c>
       <c r="I18" s="3"/>
+      <c r="K18" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="L18" s="5"/>
     </row>
     <row r="19" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="18" t="s">
@@ -1406,6 +1469,9 @@
         <v>99</v>
       </c>
       <c r="C32" s="3"/>
+      <c r="E32" s="14" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="33" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
@@ -1425,6 +1491,8 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B26:C26"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="E15:F15"/>
@@ -1440,8 +1508,6 @@
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B26:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1449,6 +1515,469 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:L36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="50.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="E2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="H2" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="24"/>
+      <c r="K2" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" s="24"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="H3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="K3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="E4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="H4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="K4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="H5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="K5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="E6" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="24"/>
+      <c r="K6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="H7" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" s="24"/>
+      <c r="K7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="E8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="H8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="E9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="H9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="K9" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="L9" s="24"/>
+    </row>
+    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="K10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="H11" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="24"/>
+      <c r="K11" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="E12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="H12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="K12" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="E13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="H13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="5"/>
+      <c r="K13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="K14" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="24"/>
+      <c r="H15" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="28"/>
+      <c r="K15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="E16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="H16" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="17"/>
+      <c r="K16" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="E17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="H17" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="17"/>
+      <c r="K17" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="H18" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" s="17"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="E19" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="24"/>
+      <c r="H19" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="19"/>
+    </row>
+    <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="24"/>
+      <c r="E21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="H21" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="31"/>
+    </row>
+    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="E22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="H22" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="17"/>
+    </row>
+    <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="H23" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23" s="17"/>
+    </row>
+    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="E24" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="24"/>
+      <c r="H24" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="17"/>
+    </row>
+    <row r="25" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="H25" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="I25" s="19"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="24"/>
+      <c r="E26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="E27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="E28" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E29" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="E30" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E31" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E32" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="20"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="20"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="H7:I7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>

</xml_diff>